<commit_message>
Nouvelle version du modèle : ajout du libellé
</commit_message>
<xml_diff>
--- a/modèle import refs constructeur.xlsx
+++ b/modèle import refs constructeur.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\francois.fabien\Downloads\Autres\Appli équivalences\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\francois.fabien\Downloads\Autres\Appli équivalences dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2788C691-2656-45CB-B9D3-A3388653E403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD2A524F-FA1C-485B-973B-3943EB7EF8CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="2640" windowWidth="21600" windowHeight="11295" xr2:uid="{26D12DEC-16C5-4501-862B-35B7F675957C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{26D12DEC-16C5-4501-862B-35B7F675957C}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>ref OEM</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Nouveau prix d'achat</t>
+  </si>
+  <si>
+    <t>libellé</t>
   </si>
 </sst>
 </file>
@@ -416,22 +419,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACEF62BB-11EE-44A2-809D-A44AA92E5A1C}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>